<commit_message>
presentacion paracapacitacion de procesos
</commit_message>
<xml_diff>
--- a/qualtcom/Organizacional/Calidad/Plan_calidad.xlsx
+++ b/qualtcom/Organizacional/Calidad/Plan_calidad.xlsx
@@ -178,7 +178,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -187,70 +187,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -319,40 +255,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -701,13 +629,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:E32"/>
+  <dimension ref="B3:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29:B31"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5"/>
     <col min="2" max="2" width="31.875"/>
@@ -718,246 +646,242 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="B3" s="1"/>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="12"/>
+      <c r="C3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="4"/>
-      <c r="C4" s="5" t="s">
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="14"/>
+      <c r="C4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+      <c r="D4" s="16"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="9"/>
-    </row>
-    <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="10" t="s">
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="10" t="s">
+      <c r="D6" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="10" t="s">
+      <c r="D7" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="s">
+      <c r="D8" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="10" t="s">
+      <c r="D9" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="10" t="s">
+      <c r="D10" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="13"/>
-      <c r="C16" s="16" t="s">
+      <c r="D11" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
+      <c r="C16" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="14"/>
-    </row>
-    <row r="17" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="15" t="s">
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="12" t="s">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="12" t="s">
+      <c r="D18" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="12" t="s">
+      <c r="D19" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="12" t="s">
+      <c r="D20" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="12" t="s">
+      <c r="D21" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="12" t="s">
+      <c r="D22" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="12" t="s">
+      <c r="D23" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:5" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="13"/>
-      <c r="C28" s="16" t="s">
+      <c r="D24" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
+      <c r="C28" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="19"/>
-      <c r="E28" s="14"/>
-    </row>
-    <row r="29" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B29" s="20" t="s">
+      <c r="D28" s="10"/>
+      <c r="E28" s="5"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D29" s="18" t="s">
+      <c r="D29" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E29" s="17" t="s">
+      <c r="E29" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="12" t="s">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E30" s="12" t="s">
+      <c r="E30" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="12" t="s">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D31" s="12" t="s">
+      <c r="D31" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E31" s="12" t="s">
+      <c r="E31" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="2:5" ht="15.75" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>